<commit_message>
create new human_9 with ankle inertia, found issue with large angular velocity
</commit_message>
<xml_diff>
--- a/six_links/sim_result.xlsx
+++ b/six_links/sim_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UCLA\lab\Exoskeleton\Dynamic Model\walkSim_ankle\six_links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376CAFBF-C35B-41F5-952B-1568E8A64EA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017FB08F-84C4-4C76-89D9-8F57D67AC7B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D99BCCEB-5C6C-4FF8-8805-D32DA5F95FDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D99BCCEB-5C6C-4FF8-8805-D32DA5F95FDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Step1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>hipLen</t>
   </si>
@@ -99,13 +99,169 @@
   </si>
   <si>
     <t>0125155756</t>
+  </si>
+  <si>
+    <t>0125164915</t>
+  </si>
+  <si>
+    <t>0125164917</t>
+  </si>
+  <si>
+    <t>0125164740</t>
+  </si>
+  <si>
+    <t>backward</t>
+  </si>
+  <si>
+    <t>0125165920</t>
+  </si>
+  <si>
+    <t>0125165731</t>
+  </si>
+  <si>
+    <t>0125170024</t>
+  </si>
+  <si>
+    <t>0125170116</t>
+  </si>
+  <si>
+    <t>human_9_load</t>
+  </si>
+  <si>
+    <t>0125170333</t>
+  </si>
+  <si>
+    <t>0125170632</t>
+  </si>
+  <si>
+    <t>0125170719</t>
+  </si>
+  <si>
+    <t>0125170652</t>
+  </si>
+  <si>
+    <t>0125170546</t>
+  </si>
+  <si>
+    <t>human_9_exo</t>
+  </si>
+  <si>
+    <t>0125170847</t>
+  </si>
+  <si>
+    <t>0125170906</t>
+  </si>
+  <si>
+    <t>0125171354</t>
+  </si>
+  <si>
+    <t>0125172015</t>
+  </si>
+  <si>
+    <t>0125172104</t>
+  </si>
+  <si>
+    <t>0125171714</t>
+  </si>
+  <si>
+    <t>0125171705</t>
+  </si>
+  <si>
+    <t>0125172041</t>
+  </si>
+  <si>
+    <t>0125171750</t>
+  </si>
+  <si>
+    <t>0125171342</t>
+  </si>
+  <si>
+    <t>0125172805</t>
+  </si>
+  <si>
+    <t>0125172548</t>
+  </si>
+  <si>
+    <t>0125172639</t>
+  </si>
+  <si>
+    <t>0125173448</t>
+  </si>
+  <si>
+    <t>0125173535</t>
+  </si>
+  <si>
+    <t>0125173307</t>
+  </si>
+  <si>
+    <t>0125174131</t>
+  </si>
+  <si>
+    <t>0125173403</t>
+  </si>
+  <si>
+    <t>0125174347</t>
+  </si>
+  <si>
+    <t>0125175118</t>
+  </si>
+  <si>
+    <t>0125175320</t>
+  </si>
+  <si>
+    <t>0125174746</t>
+  </si>
+  <si>
+    <t>0125174727</t>
+  </si>
+  <si>
+    <t>0125175247</t>
+  </si>
+  <si>
+    <t>0125183726</t>
+  </si>
+  <si>
+    <t>0125183702</t>
+  </si>
+  <si>
+    <t>0125174634</t>
+  </si>
+  <si>
+    <t>0125184505</t>
+  </si>
+  <si>
+    <t>0125184946</t>
+  </si>
+  <si>
+    <t>0125191027</t>
+  </si>
+  <si>
+    <t>0125191322</t>
+  </si>
+  <si>
+    <t>0125191228</t>
+  </si>
+  <si>
+    <t>0125190924</t>
+  </si>
+  <si>
+    <t>0125191842</t>
+  </si>
+  <si>
+    <t>0125192636</t>
+  </si>
+  <si>
+    <t>0125204223</t>
+  </si>
+  <si>
+    <t>0126012219</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,16 +269,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -130,15 +298,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,18 +637,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F459C3B4-1719-419D-9B64-04CDD9795DE1}">
-  <dimension ref="A1:AC52"/>
+  <dimension ref="A1:AE52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="2" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -478,7 +665,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -486,7 +673,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -494,7 +681,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -502,10 +689,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -537,8 +730,10 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -567,253 +762,129 @@
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+    </row>
+    <row r="9" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="10" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    </row>
+    <row r="11" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    </row>
+    <row r="12" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    </row>
+    <row r="13" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    </row>
+    <row r="14" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    </row>
+    <row r="15" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -842,8 +913,13 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
-    </row>
-    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -872,8 +948,10 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
-    </row>
-    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -902,218 +980,129 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
-    </row>
-    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-    </row>
-    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-    </row>
-    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-    </row>
-    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-      <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
-    </row>
-    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
-      <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
-    </row>
-    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
-      <c r="AB24" s="1"/>
-      <c r="AC24" s="1"/>
-    </row>
-    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
-    </row>
-    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+    </row>
+    <row r="19" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1142,8 +1131,10 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
-    </row>
-    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1172,8 +1163,10 @@
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
-    </row>
-    <row r="28" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1202,8 +1195,10 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
-    </row>
-    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1232,8 +1227,10 @@
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
-    </row>
-    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1262,8 +1259,10 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
-    </row>
-    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1292,8 +1291,10 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
-    </row>
-    <row r="32" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1322,8 +1323,10 @@
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
-    </row>
-    <row r="33" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+    </row>
+    <row r="33" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1352,8 +1355,10 @@
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
-    </row>
-    <row r="34" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+    </row>
+    <row r="34" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1382,8 +1387,10 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
-    </row>
-    <row r="35" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+    </row>
+    <row r="35" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1412,8 +1419,10 @@
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
-    </row>
-    <row r="36" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD35" s="1"/>
+      <c r="AE35" s="1"/>
+    </row>
+    <row r="36" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1442,8 +1451,10 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
-    </row>
-    <row r="37" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+    </row>
+    <row r="37" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1472,8 +1483,10 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
-    </row>
-    <row r="38" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="1"/>
+    </row>
+    <row r="38" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1502,8 +1515,10 @@
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
-    </row>
-    <row r="39" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+    </row>
+    <row r="39" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1532,8 +1547,10 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
-    </row>
-    <row r="40" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD39" s="1"/>
+      <c r="AE39" s="1"/>
+    </row>
+    <row r="40" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1562,8 +1579,10 @@
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
-    </row>
-    <row r="41" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD40" s="1"/>
+      <c r="AE40" s="1"/>
+    </row>
+    <row r="41" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1592,8 +1611,10 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
-    </row>
-    <row r="42" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD41" s="1"/>
+      <c r="AE41" s="1"/>
+    </row>
+    <row r="42" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1622,8 +1643,10 @@
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
       <c r="AC42" s="1"/>
-    </row>
-    <row r="43" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD42" s="1"/>
+      <c r="AE42" s="1"/>
+    </row>
+    <row r="43" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1652,8 +1675,10 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
-    </row>
-    <row r="44" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD43" s="1"/>
+      <c r="AE43" s="1"/>
+    </row>
+    <row r="44" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1682,8 +1707,10 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
       <c r="AC44" s="1"/>
-    </row>
-    <row r="45" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD44" s="1"/>
+      <c r="AE44" s="1"/>
+    </row>
+    <row r="45" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1712,8 +1739,10 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
       <c r="AC45" s="1"/>
-    </row>
-    <row r="46" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD45" s="1"/>
+      <c r="AE45" s="1"/>
+    </row>
+    <row r="46" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1742,8 +1771,10 @@
       <c r="AA46" s="1"/>
       <c r="AB46" s="1"/>
       <c r="AC46" s="1"/>
-    </row>
-    <row r="47" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD46" s="1"/>
+      <c r="AE46" s="1"/>
+    </row>
+    <row r="47" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1772,8 +1803,10 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
       <c r="AC47" s="1"/>
-    </row>
-    <row r="48" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD47" s="1"/>
+      <c r="AE47" s="1"/>
+    </row>
+    <row r="48" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1802,8 +1835,10 @@
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
       <c r="AC48" s="1"/>
-    </row>
-    <row r="49" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD48" s="1"/>
+      <c r="AE48" s="1"/>
+    </row>
+    <row r="49" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1832,8 +1867,10 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
       <c r="AC49" s="1"/>
-    </row>
-    <row r="50" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD49" s="1"/>
+      <c r="AE49" s="1"/>
+    </row>
+    <row r="50" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1862,8 +1899,10 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
       <c r="AC50" s="1"/>
-    </row>
-    <row r="51" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD50" s="1"/>
+      <c r="AE50" s="1"/>
+    </row>
+    <row r="51" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1892,8 +1931,10 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
-    </row>
-    <row r="52" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AD51" s="1"/>
+      <c r="AE51" s="1"/>
+    </row>
+    <row r="52" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1922,6 +1963,8 @@
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
       <c r="AC52" s="1"/>
+      <c r="AD52" s="1"/>
+      <c r="AE52" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
vel_con currently work, but requires knee tendon force
</commit_message>
<xml_diff>
--- a/six_links/sim_result.xlsx
+++ b/six_links/sim_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UCLA\lab\Exoskeleton\Dynamic Model\walkSim_ankle\six_links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017FB08F-84C4-4C76-89D9-8F57D67AC7B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEE41A1-2D23-47F4-9556-AA22754BB94E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D99BCCEB-5C6C-4FF8-8805-D32DA5F95FDE}"/>
+    <workbookView xWindow="765" yWindow="3180" windowWidth="21600" windowHeight="12735" xr2:uid="{D99BCCEB-5C6C-4FF8-8805-D32DA5F95FDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Step1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>hipLen</t>
   </si>
@@ -80,181 +80,136 @@
     <t>effKA</t>
   </si>
   <si>
-    <t>0125155926</t>
-  </si>
-  <si>
-    <t>0125160053</t>
-  </si>
-  <si>
-    <t>0125155907</t>
-  </si>
-  <si>
-    <t>0125155802</t>
-  </si>
-  <si>
-    <t>0125155852</t>
-  </si>
-  <si>
-    <t>0125155835</t>
-  </si>
-  <si>
-    <t>0125155756</t>
-  </si>
-  <si>
-    <t>0125164915</t>
-  </si>
-  <si>
-    <t>0125164917</t>
-  </si>
-  <si>
-    <t>0125164740</t>
-  </si>
-  <si>
     <t>backward</t>
   </si>
   <si>
-    <t>0125165920</t>
-  </si>
-  <si>
-    <t>0125165731</t>
-  </si>
-  <si>
-    <t>0125170024</t>
-  </si>
-  <si>
-    <t>0125170116</t>
-  </si>
-  <si>
     <t>human_9_load</t>
   </si>
   <si>
-    <t>0125170333</t>
-  </si>
-  <si>
-    <t>0125170632</t>
-  </si>
-  <si>
-    <t>0125170719</t>
-  </si>
-  <si>
-    <t>0125170652</t>
-  </si>
-  <si>
-    <t>0125170546</t>
-  </si>
-  <si>
-    <t>human_9_exo</t>
-  </si>
-  <si>
-    <t>0125170847</t>
-  </si>
-  <si>
-    <t>0125170906</t>
-  </si>
-  <si>
-    <t>0125171354</t>
-  </si>
-  <si>
-    <t>0125172015</t>
-  </si>
-  <si>
-    <t>0125172104</t>
-  </si>
-  <si>
-    <t>0125171714</t>
-  </si>
-  <si>
-    <t>0125171705</t>
-  </si>
-  <si>
-    <t>0125172041</t>
-  </si>
-  <si>
-    <t>0125171750</t>
-  </si>
-  <si>
-    <t>0125171342</t>
-  </si>
-  <si>
-    <t>0125172805</t>
-  </si>
-  <si>
-    <t>0125172548</t>
-  </si>
-  <si>
-    <t>0125172639</t>
-  </si>
-  <si>
-    <t>0125173448</t>
-  </si>
-  <si>
-    <t>0125173535</t>
-  </si>
-  <si>
-    <t>0125173307</t>
-  </si>
-  <si>
-    <t>0125174131</t>
-  </si>
-  <si>
-    <t>0125173403</t>
-  </si>
-  <si>
-    <t>0125174347</t>
-  </si>
-  <si>
-    <t>0125175118</t>
-  </si>
-  <si>
-    <t>0125175320</t>
-  </si>
-  <si>
-    <t>0125174746</t>
-  </si>
-  <si>
-    <t>0125174727</t>
-  </si>
-  <si>
-    <t>0125175247</t>
-  </si>
-  <si>
-    <t>0125183726</t>
-  </si>
-  <si>
-    <t>0125183702</t>
-  </si>
-  <si>
-    <t>0125174634</t>
-  </si>
-  <si>
-    <t>0125184505</t>
-  </si>
-  <si>
-    <t>0125184946</t>
-  </si>
-  <si>
-    <t>0125191027</t>
-  </si>
-  <si>
-    <t>0125191322</t>
-  </si>
-  <si>
-    <t>0125191228</t>
-  </si>
-  <si>
-    <t>0125190924</t>
-  </si>
-  <si>
-    <t>0125191842</t>
-  </si>
-  <si>
-    <t>0125192636</t>
-  </si>
-  <si>
-    <t>0125204223</t>
-  </si>
-  <si>
-    <t>0126012219</t>
+    <t>0206000141</t>
+  </si>
+  <si>
+    <t>0205235730</t>
+  </si>
+  <si>
+    <t>0206000110</t>
+  </si>
+  <si>
+    <t>0206000054</t>
+  </si>
+  <si>
+    <t>0206000033</t>
+  </si>
+  <si>
+    <t>0207222945</t>
+  </si>
+  <si>
+    <t>0207223949</t>
+  </si>
+  <si>
+    <t>0207223824</t>
+  </si>
+  <si>
+    <t>0207223659</t>
+  </si>
+  <si>
+    <t>0207232750</t>
+  </si>
+  <si>
+    <t>0207233003</t>
+  </si>
+  <si>
+    <t>0207233150</t>
+  </si>
+  <si>
+    <t>0207233103</t>
+  </si>
+  <si>
+    <t>0207234726</t>
+  </si>
+  <si>
+    <t>0207235429</t>
+  </si>
+  <si>
+    <t>0207235223</t>
+  </si>
+  <si>
+    <t>0207235341</t>
+  </si>
+  <si>
+    <t>0207235354</t>
+  </si>
+  <si>
+    <t>0207235425</t>
+  </si>
+  <si>
+    <t>0207235328</t>
+  </si>
+  <si>
+    <t>0207235314</t>
+  </si>
+  <si>
+    <t>0208004556</t>
+  </si>
+  <si>
+    <t>0208004533</t>
+  </si>
+  <si>
+    <t>0208004350</t>
+  </si>
+  <si>
+    <t>0208004603</t>
+  </si>
+  <si>
+    <t>0208004618</t>
+  </si>
+  <si>
+    <t>0208004310</t>
+  </si>
+  <si>
+    <t>0208004427</t>
+  </si>
+  <si>
+    <t>0208011030</t>
+  </si>
+  <si>
+    <t>0208011059</t>
+  </si>
+  <si>
+    <t>0208010942</t>
+  </si>
+  <si>
+    <t>0208010951</t>
+  </si>
+  <si>
+    <t>0208010828</t>
+  </si>
+  <si>
+    <t>0208110847</t>
+  </si>
+  <si>
+    <t>0208110754</t>
+  </si>
+  <si>
+    <t>0208111153</t>
+  </si>
+  <si>
+    <t>0208110658</t>
+  </si>
+  <si>
+    <t>0208111009</t>
+  </si>
+  <si>
+    <t>0208110907</t>
+  </si>
+  <si>
+    <t>0208112819</t>
+  </si>
+  <si>
+    <t>0208113044</t>
+  </si>
+  <si>
+    <t>0208112646</t>
   </si>
 </sst>
 </file>
@@ -637,35 +592,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F459C3B4-1719-419D-9B64-04CDD9795DE1}">
-  <dimension ref="A1:AE52"/>
+  <dimension ref="A1:AD52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="2" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+        <v>2.0754000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+        <v>2.5745</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -673,7 +628,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -681,7 +636,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -689,16 +644,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -731,9 +683,8 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -763,128 +714,106 @@
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
-    </row>
-    <row r="9" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -914,11 +843,10 @@
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
-      <c r="AE16" s="1"/>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -949,9 +877,8 @@
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
-      <c r="AE17" s="1"/>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -981,128 +908,106 @@
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
-      <c r="AE18" s="1"/>
-    </row>
-    <row r="19" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1132,9 +1037,8 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
-      <c r="AE26" s="1"/>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1164,9 +1068,8 @@
       <c r="AB27" s="1"/>
       <c r="AC27" s="1"/>
       <c r="AD27" s="1"/>
-      <c r="AE27" s="1"/>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1196,9 +1099,8 @@
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
-      <c r="AE28" s="1"/>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1228,9 +1130,8 @@
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
-      <c r="AE29" s="1"/>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1260,9 +1161,8 @@
       <c r="AB30" s="1"/>
       <c r="AC30" s="1"/>
       <c r="AD30" s="1"/>
-      <c r="AE30" s="1"/>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1292,9 +1192,8 @@
       <c r="AB31" s="1"/>
       <c r="AC31" s="1"/>
       <c r="AD31" s="1"/>
-      <c r="AE31" s="1"/>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1324,9 +1223,8 @@
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
-      <c r="AE32" s="1"/>
-    </row>
-    <row r="33" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1356,9 +1254,8 @@
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
-      <c r="AE33" s="1"/>
-    </row>
-    <row r="34" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1388,9 +1285,8 @@
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
-      <c r="AE34" s="1"/>
-    </row>
-    <row r="35" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1420,9 +1316,8 @@
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
-      <c r="AE35" s="1"/>
-    </row>
-    <row r="36" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1452,9 +1347,8 @@
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
-      <c r="AE36" s="1"/>
-    </row>
-    <row r="37" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1484,9 +1378,8 @@
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
-      <c r="AE37" s="1"/>
-    </row>
-    <row r="38" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1516,9 +1409,8 @@
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
-      <c r="AE38" s="1"/>
-    </row>
-    <row r="39" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1548,9 +1440,8 @@
       <c r="AB39" s="1"/>
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
-      <c r="AE39" s="1"/>
-    </row>
-    <row r="40" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1580,9 +1471,8 @@
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
-      <c r="AE40" s="1"/>
-    </row>
-    <row r="41" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1612,9 +1502,8 @@
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
-      <c r="AE41" s="1"/>
-    </row>
-    <row r="42" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1644,9 +1533,8 @@
       <c r="AB42" s="1"/>
       <c r="AC42" s="1"/>
       <c r="AD42" s="1"/>
-      <c r="AE42" s="1"/>
-    </row>
-    <row r="43" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1676,9 +1564,8 @@
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
       <c r="AD43" s="1"/>
-      <c r="AE43" s="1"/>
-    </row>
-    <row r="44" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1708,9 +1595,8 @@
       <c r="AB44" s="1"/>
       <c r="AC44" s="1"/>
       <c r="AD44" s="1"/>
-      <c r="AE44" s="1"/>
-    </row>
-    <row r="45" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1740,9 +1626,8 @@
       <c r="AB45" s="1"/>
       <c r="AC45" s="1"/>
       <c r="AD45" s="1"/>
-      <c r="AE45" s="1"/>
-    </row>
-    <row r="46" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1772,9 +1657,8 @@
       <c r="AB46" s="1"/>
       <c r="AC46" s="1"/>
       <c r="AD46" s="1"/>
-      <c r="AE46" s="1"/>
-    </row>
-    <row r="47" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1804,9 +1688,8 @@
       <c r="AB47" s="1"/>
       <c r="AC47" s="1"/>
       <c r="AD47" s="1"/>
-      <c r="AE47" s="1"/>
-    </row>
-    <row r="48" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1836,9 +1719,8 @@
       <c r="AB48" s="1"/>
       <c r="AC48" s="1"/>
       <c r="AD48" s="1"/>
-      <c r="AE48" s="1"/>
-    </row>
-    <row r="49" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1868,9 +1750,8 @@
       <c r="AB49" s="1"/>
       <c r="AC49" s="1"/>
       <c r="AD49" s="1"/>
-      <c r="AE49" s="1"/>
-    </row>
-    <row r="50" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1900,9 +1781,8 @@
       <c r="AB50" s="1"/>
       <c r="AC50" s="1"/>
       <c r="AD50" s="1"/>
-      <c r="AE50" s="1"/>
-    </row>
-    <row r="51" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1932,9 +1812,8 @@
       <c r="AB51" s="1"/>
       <c r="AC51" s="1"/>
       <c r="AD51" s="1"/>
-      <c r="AE51" s="1"/>
-    </row>
-    <row r="52" spans="2:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1964,7 +1843,6 @@
       <c r="AB52" s="1"/>
       <c r="AC52" s="1"/>
       <c r="AD52" s="1"/>
-      <c r="AE52" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
have initial results of human, human_load, exo
</commit_message>
<xml_diff>
--- a/six_links/sim_result.xlsx
+++ b/six_links/sim_result.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UCLA\lab\Exoskeleton\Dynamic Model\walkSim_ankle\six_links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEE41A1-2D23-47F4-9556-AA22754BB94E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C38514-8F7C-4E47-9E27-D8346DB6B653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="3180" windowWidth="21600" windowHeight="12735" xr2:uid="{D99BCCEB-5C6C-4FF8-8805-D32DA5F95FDE}"/>
+    <workbookView xWindow="32055" yWindow="3600" windowWidth="21600" windowHeight="12465" activeTab="2" xr2:uid="{D99BCCEB-5C6C-4FF8-8805-D32DA5F95FDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Step1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="144">
   <si>
     <t>hipLen</t>
   </si>
@@ -56,9 +58,6 @@
     <t>forward</t>
   </si>
   <si>
-    <t>human_9_load_exo</t>
-  </si>
-  <si>
     <t>base</t>
   </si>
   <si>
@@ -86,130 +85,388 @@
     <t>human_9_load</t>
   </si>
   <si>
-    <t>0206000141</t>
-  </si>
-  <si>
-    <t>0205235730</t>
-  </si>
-  <si>
-    <t>0206000110</t>
-  </si>
-  <si>
-    <t>0206000054</t>
-  </si>
-  <si>
-    <t>0206000033</t>
-  </si>
-  <si>
-    <t>0207222945</t>
-  </si>
-  <si>
-    <t>0207223949</t>
-  </si>
-  <si>
-    <t>0207223824</t>
-  </si>
-  <si>
-    <t>0207223659</t>
-  </si>
-  <si>
-    <t>0207232750</t>
-  </si>
-  <si>
-    <t>0207233003</t>
-  </si>
-  <si>
-    <t>0207233150</t>
-  </si>
-  <si>
-    <t>0207233103</t>
-  </si>
-  <si>
-    <t>0207234726</t>
-  </si>
-  <si>
-    <t>0207235429</t>
-  </si>
-  <si>
-    <t>0207235223</t>
-  </si>
-  <si>
-    <t>0207235341</t>
-  </si>
-  <si>
-    <t>0207235354</t>
-  </si>
-  <si>
-    <t>0207235425</t>
-  </si>
-  <si>
-    <t>0207235328</t>
-  </si>
-  <si>
-    <t>0207235314</t>
-  </si>
-  <si>
-    <t>0208004556</t>
-  </si>
-  <si>
-    <t>0208004533</t>
-  </si>
-  <si>
-    <t>0208004350</t>
-  </si>
-  <si>
-    <t>0208004603</t>
-  </si>
-  <si>
-    <t>0208004618</t>
-  </si>
-  <si>
-    <t>0208004310</t>
-  </si>
-  <si>
-    <t>0208004427</t>
-  </si>
-  <si>
-    <t>0208011030</t>
-  </si>
-  <si>
-    <t>0208011059</t>
-  </si>
-  <si>
-    <t>0208010942</t>
-  </si>
-  <si>
-    <t>0208010951</t>
-  </si>
-  <si>
-    <t>0208010828</t>
-  </si>
-  <si>
-    <t>0208110847</t>
-  </si>
-  <si>
-    <t>0208110754</t>
-  </si>
-  <si>
-    <t>0208111153</t>
-  </si>
-  <si>
-    <t>0208110658</t>
-  </si>
-  <si>
-    <t>0208111009</t>
-  </si>
-  <si>
-    <t>0208110907</t>
-  </si>
-  <si>
-    <t>0208112819</t>
-  </si>
-  <si>
-    <t>0208113044</t>
-  </si>
-  <si>
-    <t>0208112646</t>
+    <t>0208231028</t>
+  </si>
+  <si>
+    <t>0208231510</t>
+  </si>
+  <si>
+    <t>0208231440</t>
+  </si>
+  <si>
+    <t>0208225530</t>
+  </si>
+  <si>
+    <t>0208231506</t>
+  </si>
+  <si>
+    <t>0208231406</t>
+  </si>
+  <si>
+    <t>0208231441</t>
+  </si>
+  <si>
+    <t>0208235114</t>
+  </si>
+  <si>
+    <t>0208235937</t>
+  </si>
+  <si>
+    <t>0208235650</t>
+  </si>
+  <si>
+    <t>0208235643</t>
+  </si>
+  <si>
+    <t>0208235815</t>
+  </si>
+  <si>
+    <t>0208235608</t>
+  </si>
+  <si>
+    <t>0208235814</t>
+  </si>
+  <si>
+    <t>0209003203</t>
+  </si>
+  <si>
+    <t>0209003634</t>
+  </si>
+  <si>
+    <t>0209003558</t>
+  </si>
+  <si>
+    <t>0209003643</t>
+  </si>
+  <si>
+    <t>0209003649</t>
+  </si>
+  <si>
+    <t>0209003632</t>
+  </si>
+  <si>
+    <t>0209003705</t>
+  </si>
+  <si>
+    <t>0209011610</t>
+  </si>
+  <si>
+    <t>0209011919</t>
+  </si>
+  <si>
+    <t>0209011629</t>
+  </si>
+  <si>
+    <t>0209010710</t>
+  </si>
+  <si>
+    <t>0209011648</t>
+  </si>
+  <si>
+    <t>0209011543</t>
+  </si>
+  <si>
+    <t>0209012002</t>
+  </si>
+  <si>
+    <t>human_9_exo_load</t>
+  </si>
+  <si>
+    <t>0209020159</t>
+  </si>
+  <si>
+    <t>0209020136</t>
+  </si>
+  <si>
+    <t>0209020359</t>
+  </si>
+  <si>
+    <t>0209020317</t>
+  </si>
+  <si>
+    <t>0209015902</t>
+  </si>
+  <si>
+    <t>0209020527</t>
+  </si>
+  <si>
+    <t>0209020154</t>
+  </si>
+  <si>
+    <t>0209111941</t>
+  </si>
+  <si>
+    <t>0209112241</t>
+  </si>
+  <si>
+    <t>0209111650</t>
+  </si>
+  <si>
+    <t>0209112237</t>
+  </si>
+  <si>
+    <t>0209112444</t>
+  </si>
+  <si>
+    <t>0209114751</t>
+  </si>
+  <si>
+    <t>0209114438</t>
+  </si>
+  <si>
+    <t>body weight</t>
+  </si>
+  <si>
+    <t>0210003419</t>
+  </si>
+  <si>
+    <t>0210004607</t>
+  </si>
+  <si>
+    <t>0210004518</t>
+  </si>
+  <si>
+    <t>0210004625</t>
+  </si>
+  <si>
+    <t>0210004756</t>
+  </si>
+  <si>
+    <t>0210004519</t>
+  </si>
+  <si>
+    <t>0210004730</t>
+  </si>
+  <si>
+    <t>0210012642</t>
+  </si>
+  <si>
+    <t>0210012751</t>
+  </si>
+  <si>
+    <t>0210012836</t>
+  </si>
+  <si>
+    <t>0210012924</t>
+  </si>
+  <si>
+    <t>0210012944</t>
+  </si>
+  <si>
+    <t>0210012641</t>
+  </si>
+  <si>
+    <t>0210012844</t>
+  </si>
+  <si>
+    <t>0210025719</t>
+  </si>
+  <si>
+    <t>0210030028</t>
+  </si>
+  <si>
+    <t>0210025818</t>
+  </si>
+  <si>
+    <t>0210025954</t>
+  </si>
+  <si>
+    <t>0210030036</t>
+  </si>
+  <si>
+    <t>0210030010</t>
+  </si>
+  <si>
+    <t>0210025950</t>
+  </si>
+  <si>
+    <t>0210111452</t>
+  </si>
+  <si>
+    <t>0210112050</t>
+  </si>
+  <si>
+    <t>0210112034</t>
+  </si>
+  <si>
+    <t>0210112054</t>
+  </si>
+  <si>
+    <t>0210112310</t>
+  </si>
+  <si>
+    <t>0210112131</t>
+  </si>
+  <si>
+    <t>0210111922</t>
+  </si>
+  <si>
+    <t>0210125014</t>
+  </si>
+  <si>
+    <t>0210124950</t>
+  </si>
+  <si>
+    <t>0210125223</t>
+  </si>
+  <si>
+    <t>0210125228</t>
+  </si>
+  <si>
+    <t>0210125135</t>
+  </si>
+  <si>
+    <t>0210125219</t>
+  </si>
+  <si>
+    <t>0210125034</t>
+  </si>
+  <si>
+    <t>0210133328</t>
+  </si>
+  <si>
+    <t>0210133919</t>
+  </si>
+  <si>
+    <t>0210133659</t>
+  </si>
+  <si>
+    <t>0210131142</t>
+  </si>
+  <si>
+    <t>0210133616</t>
+  </si>
+  <si>
+    <t>0210133830</t>
+  </si>
+  <si>
+    <t>0210133826</t>
+  </si>
+  <si>
+    <t>0210142700</t>
+  </si>
+  <si>
+    <t>0210142617</t>
+  </si>
+  <si>
+    <t>0210142443</t>
+  </si>
+  <si>
+    <t>0210142525</t>
+  </si>
+  <si>
+    <t>0210142542</t>
+  </si>
+  <si>
+    <t>0210142610</t>
+  </si>
+  <si>
+    <t>0210142552</t>
+  </si>
+  <si>
+    <t>0210154811</t>
+  </si>
+  <si>
+    <t>0210154915</t>
+  </si>
+  <si>
+    <t>0210154638</t>
+  </si>
+  <si>
+    <t>0210155110</t>
+  </si>
+  <si>
+    <t>0210155103</t>
+  </si>
+  <si>
+    <t>0210155313</t>
+  </si>
+  <si>
+    <t>0210155106</t>
+  </si>
+  <si>
+    <t>0210170432</t>
+  </si>
+  <si>
+    <t>0210170337</t>
+  </si>
+  <si>
+    <t>0210170341</t>
+  </si>
+  <si>
+    <t>0210170523</t>
+  </si>
+  <si>
+    <t>0210170543</t>
+  </si>
+  <si>
+    <t>0210170501</t>
+  </si>
+  <si>
+    <t>0210170430</t>
+  </si>
+  <si>
+    <t>0210205434</t>
+  </si>
+  <si>
+    <t>0210205803</t>
+  </si>
+  <si>
+    <t>0210205537</t>
+  </si>
+  <si>
+    <t>0210205607</t>
+  </si>
+  <si>
+    <t>0210205513</t>
+  </si>
+  <si>
+    <t>0210205528</t>
+  </si>
+  <si>
+    <t>0210205247</t>
+  </si>
+  <si>
+    <t>0210214503</t>
+  </si>
+  <si>
+    <t>0210214547</t>
+  </si>
+  <si>
+    <t>0210214444</t>
+  </si>
+  <si>
+    <t>0210214314</t>
+  </si>
+  <si>
+    <t>0210214205</t>
+  </si>
+  <si>
+    <t>0210214534</t>
+  </si>
+  <si>
+    <t>0210214505</t>
+  </si>
+  <si>
+    <t>0210225213</t>
+  </si>
+  <si>
+    <t>0210225503</t>
+  </si>
+  <si>
+    <t>0210225332</t>
+  </si>
+  <si>
+    <t>0210224300</t>
+  </si>
+  <si>
+    <t>0210225302</t>
+  </si>
+  <si>
+    <t>0210224943</t>
+  </si>
+  <si>
+    <t>0210224515</t>
   </si>
 </sst>
 </file>
@@ -594,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F459C3B4-1719-419D-9B64-04CDD9795DE1}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,6 +868,9 @@
       <c r="B1">
         <v>2.0754000000000001</v>
       </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -619,6 +879,12 @@
       <c r="B2">
         <v>2.5745</v>
       </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>65</v>
+      </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -644,10 +910,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -717,27 +983,27 @@
     </row>
     <row r="9" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>46</v>
@@ -745,13 +1011,13 @@
     </row>
     <row r="11" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>47</v>
@@ -759,41 +1025,41 @@
     </row>
     <row r="12" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>50</v>
@@ -801,16 +1067,16 @@
     </row>
     <row r="15" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -846,7 +1112,7 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -911,100 +1177,100 @@
     </row>
     <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
@@ -1848,4 +2114,607 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FDBA239-AF0C-474C-8ACF-96DF78E496EE}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>2.1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2.8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C7CFEB-E8C0-466B-9AEB-3AB7AD6C5C4E}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
front ankle and back ankle joint pos are not continuous
</commit_message>
<xml_diff>
--- a/six_links/sim_result.xlsx
+++ b/six_links/sim_result.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UCLA\lab\Exoskeleton\Dynamic Model\walkSim_ankle\six_links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C38514-8F7C-4E47-9E27-D8346DB6B653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC50C021-F315-4C57-A33A-4045BAA32527}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32055" yWindow="3600" windowWidth="21600" windowHeight="12465" activeTab="2" xr2:uid="{D99BCCEB-5C6C-4FF8-8805-D32DA5F95FDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D99BCCEB-5C6C-4FF8-8805-D32DA5F95FDE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Step1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Nominal" sheetId="1" r:id="rId1"/>
+    <sheet name="Step1" sheetId="2" r:id="rId2"/>
+    <sheet name="Step2" sheetId="3" r:id="rId3"/>
+    <sheet name="Step3" sheetId="4" r:id="rId4"/>
+    <sheet name="Step4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="228">
   <si>
     <t>hipLen</t>
   </si>
@@ -467,6 +469,258 @@
   </si>
   <si>
     <t>0210224515</t>
+  </si>
+  <si>
+    <t>0210232117</t>
+  </si>
+  <si>
+    <t>0210235027</t>
+  </si>
+  <si>
+    <t>0210235026</t>
+  </si>
+  <si>
+    <t>0210235223</t>
+  </si>
+  <si>
+    <t>0210234829</t>
+  </si>
+  <si>
+    <t>0211002804</t>
+  </si>
+  <si>
+    <t>0210235111</t>
+  </si>
+  <si>
+    <t>0211010801</t>
+  </si>
+  <si>
+    <t>0211010454</t>
+  </si>
+  <si>
+    <t>0211014455</t>
+  </si>
+  <si>
+    <t>0211005024</t>
+  </si>
+  <si>
+    <t>0211011140</t>
+  </si>
+  <si>
+    <t>0211020146</t>
+  </si>
+  <si>
+    <t>0211020218</t>
+  </si>
+  <si>
+    <t>0211024339</t>
+  </si>
+  <si>
+    <t>0211024357</t>
+  </si>
+  <si>
+    <t>0211154459</t>
+  </si>
+  <si>
+    <t>0211024258</t>
+  </si>
+  <si>
+    <t>0211024552</t>
+  </si>
+  <si>
+    <t>0211153511</t>
+  </si>
+  <si>
+    <t>0211154414</t>
+  </si>
+  <si>
+    <t>0210235640</t>
+  </si>
+  <si>
+    <t>0211002551</t>
+  </si>
+  <si>
+    <t>0211002607</t>
+  </si>
+  <si>
+    <t>0211001604</t>
+  </si>
+  <si>
+    <t>0211002440</t>
+  </si>
+  <si>
+    <t>0211010505</t>
+  </si>
+  <si>
+    <t>0211002456</t>
+  </si>
+  <si>
+    <t>0211020007</t>
+  </si>
+  <si>
+    <t>0211020140</t>
+  </si>
+  <si>
+    <t>0211022814</t>
+  </si>
+  <si>
+    <t>0211012412</t>
+  </si>
+  <si>
+    <t>0211015833</t>
+  </si>
+  <si>
+    <t>0211024231</t>
+  </si>
+  <si>
+    <t>0211024213</t>
+  </si>
+  <si>
+    <t>0211153110</t>
+  </si>
+  <si>
+    <t>0211153522</t>
+  </si>
+  <si>
+    <t>0211173421</t>
+  </si>
+  <si>
+    <t>0211153238</t>
+  </si>
+  <si>
+    <t>0211153341</t>
+  </si>
+  <si>
+    <t>0211173535</t>
+  </si>
+  <si>
+    <t>0211173503</t>
+  </si>
+  <si>
+    <t>0211172913</t>
+  </si>
+  <si>
+    <t>0211182640</t>
+  </si>
+  <si>
+    <t>0211182639</t>
+  </si>
+  <si>
+    <t>0211182542</t>
+  </si>
+  <si>
+    <t>0211182702</t>
+  </si>
+  <si>
+    <t>0211182651</t>
+  </si>
+  <si>
+    <t>0211211103</t>
+  </si>
+  <si>
+    <t>0212023450</t>
+  </si>
+  <si>
+    <t>0212023834</t>
+  </si>
+  <si>
+    <t>0212023919</t>
+  </si>
+  <si>
+    <t>0212024002</t>
+  </si>
+  <si>
+    <t>0212024014</t>
+  </si>
+  <si>
+    <t>0212024012</t>
+  </si>
+  <si>
+    <t>0212023943</t>
+  </si>
+  <si>
+    <t>0212143405</t>
+  </si>
+  <si>
+    <t>0212160519</t>
+  </si>
+  <si>
+    <t>0212143908</t>
+  </si>
+  <si>
+    <t>0212160553</t>
+  </si>
+  <si>
+    <t>0212143548</t>
+  </si>
+  <si>
+    <t>0212143753</t>
+  </si>
+  <si>
+    <t>0212143951</t>
+  </si>
+  <si>
+    <t>0214182034</t>
+  </si>
+  <si>
+    <t>0211211138</t>
+  </si>
+  <si>
+    <t>0211211100</t>
+  </si>
+  <si>
+    <t>0211210726</t>
+  </si>
+  <si>
+    <t>0211210834</t>
+  </si>
+  <si>
+    <t>0211210723</t>
+  </si>
+  <si>
+    <t>0212014147</t>
+  </si>
+  <si>
+    <t>0212130912</t>
+  </si>
+  <si>
+    <t>0212144024</t>
+  </si>
+  <si>
+    <t>0212130654</t>
+  </si>
+  <si>
+    <t>0212151232</t>
+  </si>
+  <si>
+    <t>0212130705</t>
+  </si>
+  <si>
+    <t>0212130952</t>
+  </si>
+  <si>
+    <t>0212130655</t>
+  </si>
+  <si>
+    <t>0212160437</t>
+  </si>
+  <si>
+    <t>0212225251</t>
+  </si>
+  <si>
+    <t>0212153110</t>
+  </si>
+  <si>
+    <t>0212225117</t>
+  </si>
+  <si>
+    <t>0212160328</t>
+  </si>
+  <si>
+    <t>0212153005</t>
+  </si>
+  <si>
+    <t>0212153450</t>
   </si>
 </sst>
 </file>
@@ -851,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F459C3B4-1719-419D-9B64-04CDD9795DE1}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,10 +1434,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>52</v>
@@ -1194,10 +1448,10 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>53</v>
@@ -1208,10 +1462,10 @@
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>54</v>
@@ -1222,10 +1476,10 @@
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>55</v>
@@ -1236,10 +1490,10 @@
         <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>58</v>
@@ -1250,10 +1504,10 @@
         <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>57</v>
@@ -1264,10 +1518,10 @@
         <v>13</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>56</v>
@@ -2121,6 +2375,308 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19:D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>2.1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2.8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C7CFEB-E8C0-466B-9AEB-3AB7AD6C5C4E}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D25"/>
     </sheetView>
   </sheetViews>
@@ -2135,7 +2691,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
@@ -2146,7 +2702,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -2203,13 +2759,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>74</v>
+        <v>116</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>88</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2217,13 +2773,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2231,13 +2787,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>90</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2245,13 +2801,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>91</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,13 +2815,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>92</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2273,13 +2829,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>79</v>
+        <v>121</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>94</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2287,13 +2843,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2319,13 +2875,13 @@
         <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2333,13 +2889,13 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2347,13 +2903,13 @@
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2361,13 +2917,13 @@
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>84</v>
+        <v>127</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>98</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2375,13 +2931,13 @@
         <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2389,13 +2945,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2403,27 +2959,26 @@
         <v>13</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C7CFEB-E8C0-466B-9AEB-3AB7AD6C5C4E}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{886666DE-565E-4104-A9B4-047002880F57}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2437,7 +2992,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>2.2000000000000002</v>
+        <v>1.8</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
@@ -2448,7 +3003,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -2505,13 +3060,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2519,13 +3074,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>104</v>
+        <v>145</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2533,13 +3088,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2547,13 +3102,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>105</v>
+        <v>147</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>119</v>
+        <v>154</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2561,13 +3116,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>106</v>
+        <v>148</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2575,13 +3130,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>121</v>
+        <v>156</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2589,13 +3144,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2621,13 +3176,13 @@
         <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>109</v>
+        <v>165</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>123</v>
+        <v>172</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2635,13 +3190,13 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>110</v>
+        <v>166</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>129</v>
+        <v>173</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>137</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2649,13 +3204,13 @@
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>115</v>
+        <v>167</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>138</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2663,13 +3218,13 @@
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>111</v>
+        <v>168</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>127</v>
+        <v>175</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>139</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2677,13 +3232,13 @@
         <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>112</v>
+        <v>169</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>126</v>
+        <v>176</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>140</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2691,13 +3246,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>113</v>
+        <v>170</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>125</v>
+        <v>177</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>143</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2705,13 +3260,314 @@
         <v>13</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>114</v>
+        <v>171</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>124</v>
+        <v>178</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>141</v>
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A325FEF2-2D99-4F78-982A-43E2D34CA1C0}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1.6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>